<commit_message>
add zss-1338 client test case, files, screenshots - partial overflow - call assertFinally() after each test
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33640" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,26 +27,106 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
-  <si>
-    <t>a loooong text with right alignment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>a loooong text with left alingment</t>
   </si>
   <si>
-    <t xml:space="preserve">right </t>
+    <t>cut</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>normal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>no overflow</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a loooong text with left alingment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>no overflow, merged</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>no overflow, merged</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F5 loooong text with right alignment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F9 loooong text with right alignment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>right aligned</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal, higher</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F6 loooong text with right alignment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F7 loooong text with right alignment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F8 loooong text with right alignment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F9 loooong text with right alignment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cut next</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cut next 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -71,15 +151,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -359,40 +443,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="3"/>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="F3" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+  <mergeCells count="2">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add zss-1364 test case
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/zsscases/zss3case/src/main/webapp/WEB-INF/issue/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/zkspreadsheet/zss.test/src/main/webapp/issue3/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -110,7 +111,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -119,14 +120,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -445,17 +446,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -463,7 +464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -472,7 +473,7 @@
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -480,7 +481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -488,7 +489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="F7" s="1" t="s">
         <v>14</v>
@@ -497,7 +498,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -508,7 +509,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -516,7 +517,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -524,7 +525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -541,4 +542,16 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refix zss-1364 scroll down to un-rendered cells add a test case
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>a loooong text with left alingment</t>
   </si>
@@ -101,6 +101,12 @@
   <si>
     <t>cut next 2</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F70 loooong text with right alignment</t>
+  </si>
+  <si>
+    <t>F71 loooong text with right alignment</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -444,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,6 +538,19 @@
         <v>10</v>
       </c>
       <c r="F11" s="5"/>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D70" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -548,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
add a test case for zss-1369 a long text can overflow a frozen column
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>a loooong text with left alingment</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>F71 loooong text with right alignment</t>
+  </si>
+  <si>
+    <t>D5 loooong text with right alignment</t>
+  </si>
+  <si>
+    <t>D70 loooong text with right alignment</t>
+  </si>
+  <si>
+    <t>C1 a very loooong text left align</t>
+  </si>
+  <si>
+    <t>C69 a very loooong text left align</t>
   </si>
 </sst>
 </file>
@@ -157,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -171,6 +183,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:D71"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,12 +579,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C70" sqref="C70"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C69" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D70" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* add a test case, expected screenshot, and test sheet for ZSS-1375
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/zkspreadsheet/zss.test/src/main/webapp/issue3/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42CDC5F-633F-614D-B986-50770E3DF658}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="protected" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>a loooong text with left alingment</t>
   </si>
@@ -124,12 +126,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -137,15 +139,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -178,24 +187,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -463,20 +475,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -484,16 +496,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -501,7 +513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="33" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -509,7 +521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="3"/>
       <c r="F7" s="1" t="s">
         <v>14</v>
@@ -518,7 +530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -529,7 +541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -537,7 +549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -545,21 +557,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="F11" s="6"/>
+    </row>
+    <row r="70" spans="3:4">
       <c r="D70" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:4">
       <c r="C71" t="s">
         <v>1</v>
       </c>
@@ -578,37 +590,154 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C1" s="6" t="s">
+    <row r="1" spans="3:4">
+      <c r="C1" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:4">
       <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C69" s="6" t="s">
+    <row r="69" spans="3:4">
+      <c r="C69" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:4">
       <c r="D70" s="1" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3AB981-EC7D-4744-8C85-0DF532BA0445}">
+  <dimension ref="A1:G71"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="33" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3"/>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="70" spans="3:4">
+      <c r="D70" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4">
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
+  <mergeCells count="2">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E11:F11"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add several cells in "freeze" sheet to test merged cell, right alignment, across frozen columns
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/zkspreadsheet/zss.test/src/main/webapp/issue3/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42CDC5F-633F-614D-B986-50770E3DF658}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C796EB85-3C17-BF48-8BA1-E52F805FA6B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="freeze" sheetId="2" r:id="rId2"/>
     <sheet name="protected" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>a loooong text with left alingment</t>
   </si>
@@ -121,17 +121,26 @@
   </si>
   <si>
     <t>C69 a very loooong text left align</t>
+  </si>
+  <si>
+    <t>A10:D10 a merged cell with right alignment</t>
+  </si>
+  <si>
+    <t>C11:D11 shorter merged cell with right alignment</t>
+  </si>
+  <si>
+    <t>right alignment in left panel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -139,20 +148,20 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -178,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -191,14 +200,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -478,17 +494,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -496,16 +512,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="D2" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -513,7 +529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="33" customHeight="1">
+    <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -521,7 +537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="F7" s="1" t="s">
         <v>14</v>
@@ -530,7 +546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -541,7 +557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -549,7 +565,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -557,21 +573,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="70" spans="3:4">
+      <c r="F11" s="7"/>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D70" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="3:4">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
         <v>1</v>
       </c>
@@ -591,36 +607,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C1:D70"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C70" sqref="C70"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C1" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="3:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="3:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="9"/>
+      <c r="C11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C69" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="3:4">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D70" s="1" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="C11:D11"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -634,13 +677,13 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -648,16 +691,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="D2" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -665,7 +708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="33" customHeight="1">
+    <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -673,7 +716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="F7" s="1" t="s">
         <v>14</v>
@@ -682,7 +725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -693,7 +736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -701,7 +744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -709,21 +752,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="70" spans="3:4">
+      <c r="F11" s="7"/>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D70" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="3:4">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
add a test case for ZSS-1384
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/1338-overflow-right-align.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/zkspreadsheet/zss.test/src/main/webapp/issue3/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C796EB85-3C17-BF48-8BA1-E52F805FA6B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D419913-3C0C-D140-96C5-B075430C38A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25600" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="freeze" sheetId="2" r:id="rId2"/>
     <sheet name="protected" sheetId="3" r:id="rId3"/>
+    <sheet name="performance" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>a loooong text with left alingment</t>
   </si>
@@ -126,10 +127,13 @@
     <t>A10:D10 a merged cell with right alignment</t>
   </si>
   <si>
-    <t>C11:D11 shorter merged cell with right alignment</t>
-  </si>
-  <si>
     <t>right alignment in left panel</t>
+  </si>
+  <si>
+    <t>press 2 in this cell, it will change all cells below to trigger rendering right alignment</t>
+  </si>
+  <si>
+    <t>C11:D11 a merged cell with right alignment</t>
   </si>
 </sst>
 </file>
@@ -187,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -202,6 +206,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -211,7 +222,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,10 +526,10 @@
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6"/>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -577,10 +587,10 @@
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="7"/>
+      <c r="E11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="10"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D70" s="1" t="s">
@@ -607,11 +617,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11:D11"/>
+      <selection pane="topRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -619,35 +629,43 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="9"/>
-      <c r="C11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="8"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="I10" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="6"/>
+      <c r="C11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C12" s="7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C69" s="4" t="s">
@@ -695,10 +713,10 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6"/>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -756,10 +774,10 @@
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="7"/>
+      <c r="E11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="10"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D70" s="1" t="s">
@@ -783,4 +801,1592 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE21255C-19C0-0649-B0A6-A5C441C9F5B9}">
+  <dimension ref="A1:J50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>9</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13">
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <v>9</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <v>9</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>8</v>
+      </c>
+      <c r="I17">
+        <v>9</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <v>9</v>
+      </c>
+      <c r="J18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>9</v>
+      </c>
+      <c r="J19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <v>9</v>
+      </c>
+      <c r="J20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="H21">
+        <v>8</v>
+      </c>
+      <c r="I21">
+        <v>9</v>
+      </c>
+      <c r="J21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>7</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <v>9</v>
+      </c>
+      <c r="J22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>8</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="J23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>8</v>
+      </c>
+      <c r="I24">
+        <v>9</v>
+      </c>
+      <c r="J24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+      <c r="J25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>7</v>
+      </c>
+      <c r="H26">
+        <v>8</v>
+      </c>
+      <c r="I26">
+        <v>9</v>
+      </c>
+      <c r="J26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>7</v>
+      </c>
+      <c r="H27">
+        <v>8</v>
+      </c>
+      <c r="I27">
+        <v>9</v>
+      </c>
+      <c r="J27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>7</v>
+      </c>
+      <c r="H28">
+        <v>8</v>
+      </c>
+      <c r="I28">
+        <v>9</v>
+      </c>
+      <c r="J28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <v>8</v>
+      </c>
+      <c r="I29">
+        <v>9</v>
+      </c>
+      <c r="J29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <v>8</v>
+      </c>
+      <c r="I30">
+        <v>9</v>
+      </c>
+      <c r="J30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>7</v>
+      </c>
+      <c r="H31">
+        <v>8</v>
+      </c>
+      <c r="I31">
+        <v>9</v>
+      </c>
+      <c r="J31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>7</v>
+      </c>
+      <c r="H32">
+        <v>8</v>
+      </c>
+      <c r="I32">
+        <v>9</v>
+      </c>
+      <c r="J32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>7</v>
+      </c>
+      <c r="H33">
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <v>9</v>
+      </c>
+      <c r="J33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>7</v>
+      </c>
+      <c r="H34">
+        <v>8</v>
+      </c>
+      <c r="I34">
+        <v>9</v>
+      </c>
+      <c r="J34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>7</v>
+      </c>
+      <c r="H35">
+        <v>8</v>
+      </c>
+      <c r="I35">
+        <v>9</v>
+      </c>
+      <c r="J35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+      <c r="G36">
+        <v>7</v>
+      </c>
+      <c r="H36">
+        <v>8</v>
+      </c>
+      <c r="I36">
+        <v>9</v>
+      </c>
+      <c r="J36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>6</v>
+      </c>
+      <c r="G37">
+        <v>7</v>
+      </c>
+      <c r="H37">
+        <v>8</v>
+      </c>
+      <c r="I37">
+        <v>9</v>
+      </c>
+      <c r="J37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>6</v>
+      </c>
+      <c r="G38">
+        <v>7</v>
+      </c>
+      <c r="H38">
+        <v>8</v>
+      </c>
+      <c r="I38">
+        <v>9</v>
+      </c>
+      <c r="J38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <v>7</v>
+      </c>
+      <c r="H39">
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <v>9</v>
+      </c>
+      <c r="J39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>6</v>
+      </c>
+      <c r="G40">
+        <v>7</v>
+      </c>
+      <c r="H40">
+        <v>8</v>
+      </c>
+      <c r="I40">
+        <v>9</v>
+      </c>
+      <c r="J40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>6</v>
+      </c>
+      <c r="G41">
+        <v>7</v>
+      </c>
+      <c r="H41">
+        <v>8</v>
+      </c>
+      <c r="I41">
+        <v>9</v>
+      </c>
+      <c r="J41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>6</v>
+      </c>
+      <c r="G42">
+        <v>7</v>
+      </c>
+      <c r="H42">
+        <v>8</v>
+      </c>
+      <c r="I42">
+        <v>9</v>
+      </c>
+      <c r="J42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>6</v>
+      </c>
+      <c r="G43">
+        <v>7</v>
+      </c>
+      <c r="H43">
+        <v>8</v>
+      </c>
+      <c r="I43">
+        <v>9</v>
+      </c>
+      <c r="J43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>6</v>
+      </c>
+      <c r="G44">
+        <v>7</v>
+      </c>
+      <c r="H44">
+        <v>8</v>
+      </c>
+      <c r="I44">
+        <v>9</v>
+      </c>
+      <c r="J44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>6</v>
+      </c>
+      <c r="G45">
+        <v>7</v>
+      </c>
+      <c r="H45">
+        <v>8</v>
+      </c>
+      <c r="I45">
+        <v>9</v>
+      </c>
+      <c r="J45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <v>6</v>
+      </c>
+      <c r="G46">
+        <v>7</v>
+      </c>
+      <c r="H46">
+        <v>8</v>
+      </c>
+      <c r="I46">
+        <v>9</v>
+      </c>
+      <c r="J46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <v>6</v>
+      </c>
+      <c r="G47">
+        <v>7</v>
+      </c>
+      <c r="H47">
+        <v>8</v>
+      </c>
+      <c r="I47">
+        <v>9</v>
+      </c>
+      <c r="J47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48">
+        <v>6</v>
+      </c>
+      <c r="G48">
+        <v>7</v>
+      </c>
+      <c r="H48">
+        <v>8</v>
+      </c>
+      <c r="I48">
+        <v>9</v>
+      </c>
+      <c r="J48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49">
+        <v>6</v>
+      </c>
+      <c r="G49">
+        <v>7</v>
+      </c>
+      <c r="H49">
+        <v>8</v>
+      </c>
+      <c r="I49">
+        <v>9</v>
+      </c>
+      <c r="J49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="E50">
+        <v>5</v>
+      </c>
+      <c r="F50">
+        <v>6</v>
+      </c>
+      <c r="G50">
+        <v>7</v>
+      </c>
+      <c r="H50">
+        <v>8</v>
+      </c>
+      <c r="I50">
+        <v>9</v>
+      </c>
+      <c r="J50">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>